<commit_message>
update dataset, support duplicate header keys, load per-food constraint data, use each item
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="31160" windowHeight="21100" tabRatio="500" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="common foods" sheetId="4" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Constraints C" sheetId="16" r:id="rId7"/>
     <sheet name="food prices" sheetId="1" r:id="rId8"/>
     <sheet name="sample food price data" sheetId="15" r:id="rId9"/>
+    <sheet name="Food prices to use" sheetId="18" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'sample food price data'!$AD$2:$BK$28</definedName>
@@ -174,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3736" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4076" uniqueCount="744">
   <si>
     <t>country</t>
   </si>
@@ -2997,7 +2998,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="647">
+  <cellStyleXfs count="673">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3645,8 +3646,34 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="381">
+  <cellXfs count="384">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4481,6 +4508,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="51" applyFont="1"/>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="74" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="51" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="51" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="51" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4493,9 +4528,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="51" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="74" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="647">
+  <cellStyles count="673">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4816,6 +4850,19 @@
     <cellStyle name="Followed Hyperlink" xfId="642" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="664" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="666" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="668" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="670" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="672" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5136,6 +5183,19 @@
     <cellStyle name="Hyperlink" xfId="641" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="645" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="647" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="649" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="651" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="653" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="655" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="661" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="663" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="665" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="667" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="669" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="671" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="51"/>
     <cellStyle name="Normal 2 2" xfId="52"/>
@@ -5719,7 +5779,7 @@
   <dimension ref="A1:G113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D114" sqref="D114"/>
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8332,13 +8392,1701 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor theme="3" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:D126"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18" style="9" customWidth="1"/>
+    <col min="2" max="2" width="39.5" style="9" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="377" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="50" customFormat="1">
+      <c r="A1" s="54" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="364" customFormat="1">
+      <c r="A2" s="344" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="68" t="s">
+        <v>234</v>
+      </c>
+      <c r="D2" s="379">
+        <v>0.36600000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>235</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.32566666666666672</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="68" t="s">
+        <v>236</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.7326666666666668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>237</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.59933333333333338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="68" t="s">
+        <v>238</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.57900000000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="68" t="s">
+        <v>239</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.61599999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="68" t="s">
+        <v>240</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.34933333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>241</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.39900000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>242</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.32276422764227641</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="68" t="s">
+        <v>243</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.5808333333333332</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="364" customFormat="1">
+      <c r="A12" s="344" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>244</v>
+      </c>
+      <c r="D12" s="379">
+        <v>1.6511257124368452</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="77" t="s">
+        <v>245</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.53329277910466721</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>246</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.17854373771380763</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="77" t="s">
+        <v>247</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.1928838951310861</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="68" t="s">
+        <v>248</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.27566666666666667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="77" t="s">
+        <v>249</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.28423990316248532</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>647</v>
+      </c>
+      <c r="C18" s="68" t="s">
+        <v>250</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="77" t="s">
+        <v>251</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.53266666666666673</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="68" t="s">
+        <v>252</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.61704941406799929</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="68" t="s">
+        <v>254</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.20859524487592118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="77" t="s">
+        <v>255</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="68" t="s">
+        <v>256</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="77" t="s">
+        <v>257</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1.1289999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="77" t="s">
+        <v>261</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="68" t="s">
+        <v>262</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="77" t="s">
+        <v>263</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="68" t="s">
+        <v>649</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="77" t="s">
+        <v>650</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="77" t="s">
+        <v>651</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.22514444444444445</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="68" t="s">
+        <v>652</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="77" t="s">
+        <v>653</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.26165097142430493</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="364" customFormat="1">
+      <c r="A33" s="344" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="68" t="s">
+        <v>269</v>
+      </c>
+      <c r="D33" s="379">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="68" t="s">
+        <v>270</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="68" t="s">
+        <v>271</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="68" t="s">
+        <v>272</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C37" s="68" t="s">
+        <v>273</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" s="68" t="s">
+        <v>274</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" s="68" t="s">
+        <v>275</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="C40" s="68" t="s">
+        <v>276</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="68" t="s">
+        <v>277</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="C42" s="68" t="s">
+        <v>278</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="68" t="s">
+        <v>279</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="C44" s="68" t="s">
+        <v>280</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" s="68" t="s">
+        <v>281</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="68" t="s">
+        <v>630</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="C47" s="68" t="s">
+        <v>631</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="C48" s="68" t="s">
+        <v>654</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="C49" s="68" t="s">
+        <v>655</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C50" s="68" t="s">
+        <v>656</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" s="68" t="s">
+        <v>657</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C52" s="68" t="s">
+        <v>658</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C53" s="68" t="s">
+        <v>659</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="364" customFormat="1">
+      <c r="A54" s="344" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" s="346" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" s="79" t="s">
+        <v>632</v>
+      </c>
+      <c r="D54" s="379">
+        <v>0.78600000000000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="68" t="s">
+        <v>660</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0.78600000000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" s="79" t="s">
+        <v>661</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.15316666666666667</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" s="68" t="s">
+        <v>662</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.15316666666666667</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C58" s="79" t="s">
+        <v>663</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0.42633333333333329</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C59" s="68" t="s">
+        <v>664</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0.46600000000000003</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C60" s="79" t="s">
+        <v>665</v>
+      </c>
+      <c r="D60" s="2">
+        <v>1.0639999999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" s="364" customFormat="1">
+      <c r="A61" s="49" t="s">
+        <v>233</v>
+      </c>
+      <c r="B61" s="345" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" s="77" t="s">
+        <v>297</v>
+      </c>
+      <c r="D61" s="379">
+        <v>0.50656565656565655</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" s="77" t="s">
+        <v>298</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1.0293333333333334</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C63" s="77" t="s">
+        <v>299</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1.7156666666666667</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C64" s="77" t="s">
+        <v>300</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1.7989999999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="C65" s="77" t="s">
+        <v>301</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C66" s="77" t="s">
+        <v>302</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C67" s="77" t="s">
+        <v>303</v>
+      </c>
+      <c r="D67" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C68" s="77" t="s">
+        <v>304</v>
+      </c>
+      <c r="D68" s="2">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C69" s="77" t="s">
+        <v>305</v>
+      </c>
+      <c r="D69" s="2">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C70" s="77" t="s">
+        <v>306</v>
+      </c>
+      <c r="D70" s="2">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C71" s="77" t="s">
+        <v>307</v>
+      </c>
+      <c r="D71" s="2">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C72" s="77" t="s">
+        <v>308</v>
+      </c>
+      <c r="D72" s="2">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C73" s="77" t="s">
+        <v>309</v>
+      </c>
+      <c r="D73" s="2">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C74" s="77" t="s">
+        <v>633</v>
+      </c>
+      <c r="D74" s="2">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>645</v>
+      </c>
+      <c r="C75" s="77" t="s">
+        <v>634</v>
+      </c>
+      <c r="D75" s="2">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C76" s="77" t="s">
+        <v>635</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C77" s="77" t="s">
+        <v>636</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>737</v>
+      </c>
+      <c r="C78" s="77" t="s">
+        <v>646</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C79" s="77" t="s">
+        <v>666</v>
+      </c>
+      <c r="D79" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C80" s="77" t="s">
+        <v>667</v>
+      </c>
+      <c r="D80" s="2">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C81" s="77" t="s">
+        <v>668</v>
+      </c>
+      <c r="D81" s="2">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C82" s="77" t="s">
+        <v>669</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C83" s="77" t="s">
+        <v>670</v>
+      </c>
+      <c r="D83" s="2">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="C84" s="77" t="s">
+        <v>671</v>
+      </c>
+      <c r="D84" s="2">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" s="364" customFormat="1">
+      <c r="A85" s="344" t="s">
+        <v>141</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C85" s="68" t="s">
+        <v>672</v>
+      </c>
+      <c r="D85" s="379">
+        <v>0.64533333333333331</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" s="364" customFormat="1">
+      <c r="A86" s="344" t="s">
+        <v>141</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C86" s="68" t="s">
+        <v>673</v>
+      </c>
+      <c r="D86" s="379">
+        <v>0.43866666666666659</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" s="364" customFormat="1">
+      <c r="A87" s="344" t="s">
+        <v>141</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C87" s="68" t="s">
+        <v>674</v>
+      </c>
+      <c r="D87" s="379">
+        <v>0.95933333333333337</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" s="364" customFormat="1">
+      <c r="A88" s="344" t="s">
+        <v>141</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C88" s="68" t="s">
+        <v>675</v>
+      </c>
+      <c r="D88" s="379">
+        <v>0.24466666666666667</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" s="364" customFormat="1">
+      <c r="A89" s="344" t="s">
+        <v>146</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C89" s="68" t="s">
+        <v>676</v>
+      </c>
+      <c r="D89" s="379">
+        <v>1.5149999999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" s="364" customFormat="1">
+      <c r="A90" s="344" t="s">
+        <v>146</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C90" s="68" t="s">
+        <v>677</v>
+      </c>
+      <c r="D90" s="379">
+        <v>0.96396574440052696</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" s="364" customFormat="1">
+      <c r="A91" s="344" t="s">
+        <v>146</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C91" s="68" t="s">
+        <v>678</v>
+      </c>
+      <c r="D91" s="379">
+        <v>0.20466666666666666</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" s="364" customFormat="1">
+      <c r="A92" s="344" t="s">
+        <v>146</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C92" s="68" t="s">
+        <v>679</v>
+      </c>
+      <c r="D92" s="379">
+        <v>1.2450396825396826</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" s="364" customFormat="1">
+      <c r="A93" s="344" t="s">
+        <v>146</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C93" s="68" t="s">
+        <v>680</v>
+      </c>
+      <c r="D93" s="379">
+        <v>1.0377777777777777</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" s="364" customFormat="1">
+      <c r="A94" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C94" s="68" t="s">
+        <v>681</v>
+      </c>
+      <c r="D94" s="379">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" s="364" customFormat="1">
+      <c r="A95" s="344" t="s">
+        <v>214</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="C95" s="68" t="s">
+        <v>682</v>
+      </c>
+      <c r="D95" s="379">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" s="364" customFormat="1">
+      <c r="A96" s="344" t="s">
+        <v>214</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C96" s="68" t="s">
+        <v>683</v>
+      </c>
+      <c r="D96" s="379">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" s="364" customFormat="1">
+      <c r="A97" s="344" t="s">
+        <v>214</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C97" s="68" t="s">
+        <v>684</v>
+      </c>
+      <c r="D97" s="379">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" s="364" customFormat="1">
+      <c r="A98" s="344" t="s">
+        <v>214</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C98" s="68" t="s">
+        <v>685</v>
+      </c>
+      <c r="D98" s="379">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" s="364" customFormat="1">
+      <c r="A99" s="344" t="s">
+        <v>214</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C99" s="68" t="s">
+        <v>686</v>
+      </c>
+      <c r="D99" s="379">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" s="364" customFormat="1">
+      <c r="A100" s="344" t="s">
+        <v>214</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C100" s="68" t="s">
+        <v>687</v>
+      </c>
+      <c r="D100" s="379">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" s="364" customFormat="1">
+      <c r="A101" s="344" t="s">
+        <v>160</v>
+      </c>
+      <c r="B101" s="346" t="s">
+        <v>161</v>
+      </c>
+      <c r="C101" s="79" t="s">
+        <v>688</v>
+      </c>
+      <c r="D101" s="379">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" s="364" customFormat="1">
+      <c r="A102" s="344" t="s">
+        <v>160</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C102" s="68" t="s">
+        <v>689</v>
+      </c>
+      <c r="D102" s="379">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" s="364" customFormat="1">
+      <c r="A103" s="344" t="s">
+        <v>160</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C103" s="79" t="s">
+        <v>690</v>
+      </c>
+      <c r="D103" s="379">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" s="364" customFormat="1">
+      <c r="A104" s="344" t="s">
+        <v>160</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C104" s="68" t="s">
+        <v>691</v>
+      </c>
+      <c r="D104" s="379">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" s="364" customFormat="1">
+      <c r="A105" s="344" t="s">
+        <v>160</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C105" s="79" t="s">
+        <v>692</v>
+      </c>
+      <c r="D105" s="379">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" s="364" customFormat="1">
+      <c r="A106" s="344" t="s">
+        <v>160</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C106" s="68" t="s">
+        <v>693</v>
+      </c>
+      <c r="D106" s="379">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" s="364" customFormat="1">
+      <c r="A107" s="344" t="s">
+        <v>167</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C107" s="68" t="s">
+        <v>694</v>
+      </c>
+      <c r="D107" s="379">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" s="364" customFormat="1">
+      <c r="A108" s="344" t="s">
+        <v>167</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C108" s="68" t="s">
+        <v>695</v>
+      </c>
+      <c r="D108" s="379">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" s="364" customFormat="1">
+      <c r="A109" s="344" t="s">
+        <v>167</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C109" s="68" t="s">
+        <v>696</v>
+      </c>
+      <c r="D109" s="379">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" s="364" customFormat="1">
+      <c r="A110" s="344" t="s">
+        <v>167</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C110" s="68" t="s">
+        <v>697</v>
+      </c>
+      <c r="D110" s="379">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" s="364" customFormat="1">
+      <c r="A111" s="344" t="s">
+        <v>167</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C111" s="68" t="s">
+        <v>698</v>
+      </c>
+      <c r="D111" s="379">
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" s="364" customFormat="1">
+      <c r="A112" s="344" t="s">
+        <v>175</v>
+      </c>
+      <c r="B112" s="345" t="s">
+        <v>176</v>
+      </c>
+      <c r="C112" s="77" t="s">
+        <v>718</v>
+      </c>
+      <c r="D112" s="379">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" s="364" customFormat="1">
+      <c r="A113" s="344" t="s">
+        <v>175</v>
+      </c>
+      <c r="B113" s="345" t="s">
+        <v>177</v>
+      </c>
+      <c r="C113" s="77" t="s">
+        <v>699</v>
+      </c>
+      <c r="D113" s="379">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" s="364" customFormat="1">
+      <c r="A114" s="23"/>
+      <c r="B114" s="23"/>
+      <c r="C114" s="378"/>
+      <c r="D114" s="379"/>
+    </row>
+    <row r="115" spans="1:4" s="364" customFormat="1">
+      <c r="A115" s="23"/>
+      <c r="B115" s="23"/>
+      <c r="C115" s="378"/>
+      <c r="D115" s="379"/>
+    </row>
+    <row r="116" spans="1:4" s="364" customFormat="1">
+      <c r="A116" s="23"/>
+      <c r="B116" s="23"/>
+      <c r="C116" s="378"/>
+      <c r="D116" s="379"/>
+    </row>
+    <row r="117" spans="1:4" s="364" customFormat="1">
+      <c r="A117" s="23"/>
+      <c r="B117" s="23"/>
+      <c r="C117" s="378"/>
+      <c r="D117" s="379"/>
+    </row>
+    <row r="118" spans="1:4" s="364" customFormat="1">
+      <c r="A118" s="23"/>
+      <c r="B118" s="23"/>
+      <c r="C118" s="378"/>
+      <c r="D118" s="379"/>
+    </row>
+    <row r="119" spans="1:4" s="364" customFormat="1">
+      <c r="A119" s="23"/>
+      <c r="B119" s="23"/>
+      <c r="C119" s="378"/>
+      <c r="D119" s="379"/>
+    </row>
+    <row r="120" spans="1:4" s="364" customFormat="1">
+      <c r="A120" s="23"/>
+      <c r="B120" s="23"/>
+      <c r="C120" s="378"/>
+      <c r="D120" s="379"/>
+    </row>
+    <row r="121" spans="1:4" s="364" customFormat="1">
+      <c r="A121" s="23"/>
+      <c r="B121" s="23"/>
+      <c r="C121" s="378"/>
+      <c r="D121" s="379"/>
+    </row>
+    <row r="122" spans="1:4" s="364" customFormat="1">
+      <c r="A122" s="23"/>
+      <c r="B122" s="23"/>
+      <c r="C122" s="378"/>
+      <c r="D122" s="379"/>
+    </row>
+    <row r="123" spans="1:4" s="364" customFormat="1">
+      <c r="A123" s="23"/>
+      <c r="B123" s="23"/>
+      <c r="C123" s="378"/>
+      <c r="D123" s="379"/>
+    </row>
+    <row r="124" spans="1:4" s="364" customFormat="1">
+      <c r="A124" s="23"/>
+      <c r="B124" s="23"/>
+      <c r="C124" s="378"/>
+      <c r="D124" s="379"/>
+    </row>
+    <row r="125" spans="1:4" s="364" customFormat="1">
+      <c r="A125" s="23"/>
+      <c r="B125" s="23"/>
+      <c r="C125" s="378"/>
+      <c r="D125" s="379"/>
+    </row>
+    <row r="126" spans="1:4" s="364" customFormat="1">
+      <c r="A126" s="23"/>
+      <c r="B126" s="23"/>
+      <c r="C126" s="378"/>
+      <c r="D126" s="379"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -9262,10 +11010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N178"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="560" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -13901,9 +15646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -15912,12 +17655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -15935,7 +17673,7 @@
     <col min="14" max="16384" width="10.83203125" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="40" customFormat="1" hidden="1">
+    <row r="1" spans="1:13" s="40" customFormat="1">
       <c r="A1" s="40" t="s">
         <v>639</v>
       </c>
@@ -15964,7 +17702,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1">
+    <row r="2" spans="1:13">
       <c r="A2" s="34" t="s">
         <v>199</v>
       </c>
@@ -15993,7 +17731,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1">
+    <row r="3" spans="1:13">
       <c r="A3" s="34" t="s">
         <v>202</v>
       </c>
@@ -16022,7 +17760,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1">
+    <row r="4" spans="1:13">
       <c r="A4" s="34" t="s">
         <v>207</v>
       </c>
@@ -16051,7 +17789,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1">
+    <row r="5" spans="1:13">
       <c r="A5" s="34" t="s">
         <v>208</v>
       </c>
@@ -16080,9 +17818,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1"/>
-    <row r="7" spans="1:13" hidden="1"/>
-    <row r="8" spans="1:13" s="42" customFormat="1" ht="30" hidden="1">
+    <row r="8" spans="1:13" s="42" customFormat="1" ht="30">
       <c r="A8" s="41" t="s">
         <v>640</v>
       </c>
@@ -16123,7 +17859,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1">
+    <row r="9" spans="1:13">
       <c r="A9" s="35" t="s">
         <v>199</v>
       </c>
@@ -16164,7 +17900,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1">
+    <row r="10" spans="1:13">
       <c r="A10" s="35" t="s">
         <v>202</v>
       </c>
@@ -16205,7 +17941,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1">
+    <row r="11" spans="1:13">
       <c r="A11" s="35" t="s">
         <v>211</v>
       </c>
@@ -16246,7 +17982,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1">
+    <row r="12" spans="1:13">
       <c r="A12" s="35" t="s">
         <v>212</v>
       </c>
@@ -16341,7 +18077,7 @@
       <c r="F16" s="34">
         <v>0</v>
       </c>
-      <c r="G16" s="380">
+      <c r="G16" s="376">
         <f>G2-(G2*0.015)</f>
         <v>17.73</v>
       </c>
@@ -16372,7 +18108,7 @@
       <c r="F17" s="34">
         <v>76</v>
       </c>
-      <c r="G17" s="380">
+      <c r="G17" s="376">
         <f>G2+(G2*0.5)</f>
         <v>27</v>
       </c>
@@ -16403,7 +18139,7 @@
       <c r="F18" s="34">
         <v>0</v>
       </c>
-      <c r="G18" s="380">
+      <c r="G18" s="376">
         <f>G3-(G3*0.015)</f>
         <v>27.58</v>
       </c>
@@ -16434,7 +18170,7 @@
       <c r="F19" s="34">
         <v>39</v>
       </c>
-      <c r="G19" s="380">
+      <c r="G19" s="376">
         <f>G3+(G3*0.5)</f>
         <v>42</v>
       </c>
@@ -16465,7 +18201,7 @@
       <c r="F20" s="34">
         <v>0</v>
       </c>
-      <c r="G20" s="380">
+      <c r="G20" s="376">
         <f>G4-(G4*0.015)</f>
         <v>24.625</v>
       </c>
@@ -16496,7 +18232,7 @@
       <c r="F21" s="34">
         <v>52</v>
       </c>
-      <c r="G21" s="380">
+      <c r="G21" s="376">
         <f>G4+(G4*0.5)</f>
         <v>37.5</v>
       </c>
@@ -16527,7 +18263,7 @@
       <c r="F22" s="34">
         <v>0</v>
       </c>
-      <c r="G22" s="380">
+      <c r="G22" s="376">
         <f>G5-(G5*0.015)</f>
         <v>29.55</v>
       </c>
@@ -16558,7 +18294,7 @@
       <c r="F23" s="34">
         <v>66</v>
       </c>
-      <c r="G23" s="380">
+      <c r="G23" s="376">
         <f>G5+(G5*0.5)</f>
         <v>45</v>
       </c>
@@ -17062,11 +18798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD131"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1160" activePane="bottomLeft"/>
-      <selection activeCell="H1" sqref="H1:H1048576"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -17098,26 +18830,26 @@
       </c>
       <c r="B2" s="94"/>
       <c r="D2" s="321"/>
-      <c r="E2" s="376" t="s">
+      <c r="E2" s="380" t="s">
         <v>224</v>
       </c>
-      <c r="F2" s="377"/>
-      <c r="G2" s="377"/>
-      <c r="H2" s="378" t="s">
+      <c r="F2" s="381"/>
+      <c r="G2" s="381"/>
+      <c r="H2" s="382" t="s">
         <v>225</v>
       </c>
-      <c r="I2" s="379"/>
-      <c r="J2" s="379"/>
-      <c r="K2" s="376" t="s">
+      <c r="I2" s="383"/>
+      <c r="J2" s="383"/>
+      <c r="K2" s="380" t="s">
         <v>227</v>
       </c>
-      <c r="L2" s="377"/>
-      <c r="M2" s="377"/>
-      <c r="N2" s="378" t="s">
+      <c r="L2" s="381"/>
+      <c r="M2" s="381"/>
+      <c r="N2" s="382" t="s">
         <v>228</v>
       </c>
-      <c r="O2" s="379"/>
-      <c r="P2" s="379"/>
+      <c r="O2" s="383"/>
+      <c r="P2" s="383"/>
     </row>
     <row r="3" spans="1:30">
       <c r="A3" s="94" t="s">
@@ -21999,9 +23731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC163"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -31543,8 +33273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="W47" sqref="W47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -33904,9 +35634,7 @@
   </sheetPr>
   <dimension ref="A1:BP143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView topLeftCell="BE1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>